<commit_message>
Zapis plików pomocniczych do poprzedniego commitu
</commit_message>
<xml_diff>
--- a/pomocnicze/Analiza_demograficzna_do opisu badania ilościowego.xlsx
+++ b/pomocnicze/Analiza_demograficzna_do opisu badania ilościowego.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPSZ\Desktop\STUDIA\doktorat_git\pomocnicze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A33DAE6-3FEB-4EAB-AF2C-629AE8D68BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BEE60F1-9F4D-4B3E-A0CB-0F5A56F88B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="-16020" windowWidth="17300" windowHeight="9850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
-  <si>
-    <t xml:space="preserve">P O L S K A ...... </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>powyżej 65 lat</t>
   </si>
@@ -88,12 +85,45 @@
   </si>
   <si>
     <t>Cała populacja Polska pow. 18 roku życia w 2020 r.</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>10-14lat</t>
+  </si>
+  <si>
+    <t>5-9lat</t>
+  </si>
+  <si>
+    <t>0-4lat</t>
+  </si>
+  <si>
+    <t>suma kontrolna</t>
+  </si>
+  <si>
+    <t>0-18</t>
+  </si>
+  <si>
+    <t>Ludność Polski w dniu 31 grudnia2020</t>
+  </si>
+  <si>
+    <t>pow 25 lat</t>
+  </si>
+  <si>
+    <t>szacunkowa wartość współczynnika skolaryzacji netto dla grupy wiekowej 19-26 lat</t>
+  </si>
+  <si>
+    <t>Oszacowanie struktury populacji badanej absolwentów i studentów wg wybranych grup wiekowych</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,9 +161,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -141,6 +172,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -422,465 +456,604 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C270"/>
+  <dimension ref="A1:G270"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B12" sqref="B12:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.73046875" customWidth="1"/>
     <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1">
         <v>38265013</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <f>$C$74</f>
+        <v>30957915</v>
+      </c>
+      <c r="D3" s="2">
+        <f>C3/C2</f>
+        <v>0.80903970945991843</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="3">
+        <f>C4/$C$74</f>
+        <v>0.21255611044865264</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <f>SUM(C63:C73)</f>
+        <v>6580294</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1">
+        <f>SUM(C4:C8)</f>
+        <v>28189155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="3">
+        <f>C5/$C$74</f>
+        <v>0.16452600247788005</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <f>SUM(C57:C62)</f>
+        <v>5093382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="3">
+        <f>C6/$C$74</f>
+        <v>0.15642222675525791</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <f>SUM(C51:C56)</f>
+        <v>4842506</v>
+      </c>
+      <c r="F6" s="7">
+        <f>7.6/28.2</f>
+        <v>0.26950354609929078</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
+        <f>C7/$C$74</f>
+        <v>0.20192826293372793</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <f>SUM(C45:C50)</f>
+        <v>6251278</v>
+      </c>
+      <c r="F7" s="8">
+        <f>ROUND(F6,2)</f>
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="3">
+        <f>C8/$C$74</f>
+        <v>0.17513114174517244</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <f>SUM(C39:C44)</f>
+        <v>5421695</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="3">
+        <f>C9/$C$74</f>
+        <v>0.10433415816278326</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(C36:C39)</f>
+        <v>3229968</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C11" s="1">
+        <f>SUM(C13:C18)</f>
+        <v>8773858</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <f>INT(C4*$F$7)</f>
+        <v>1776679</v>
+      </c>
+      <c r="D13" s="3">
+        <f>C13/$C$11</f>
+        <v>0.20249689475257066</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14:C18" si="0">INT(C5*$F$7)</f>
+        <v>1375213</v>
+      </c>
+      <c r="D14" s="3">
+        <f>C14/$C$11</f>
+        <v>0.15673982870477274</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>1307476</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15/$C$11</f>
+        <v>0.14901950772396819</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>1687845</v>
+      </c>
+      <c r="D16" s="3">
+        <f>C16/$C$11</f>
+        <v>0.19237204431619476</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>1463857</v>
+      </c>
+      <c r="D17" s="3">
+        <f>C17/$C$11</f>
+        <v>0.16684302390123024</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <f>INT(C9*$F$11)</f>
+        <v>1162788</v>
+      </c>
+      <c r="D18" s="3">
+        <f>C18/$C$11</f>
+        <v>0.13252870060126343</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <f>SUM(C32:C35)-C36</f>
+        <v>7307098</v>
+      </c>
+      <c r="D30">
+        <f>C30/C2</f>
+        <v>0.19096029054008162</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31">
+        <f>SUM(C32:C73)-C36</f>
+        <v>38265013</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32">
+        <v>1902236</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33">
+        <v>1910470</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34">
+        <v>2065628</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1">
-        <f>$C$53</f>
-        <v>30957915</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
-        <f>C4/$C$53</f>
-        <v>0.21255611044865264</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <f>SUM(C42:C52)</f>
-        <v>6580294</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
-        <f t="shared" ref="A5:A9" si="0">C5/$C$53</f>
-        <v>0.16452600247788005</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <f>SUM(C36:C41)</f>
-        <v>5093382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15642222675525791</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1">
-        <f>SUM(C30:C35)</f>
-        <v>4842506</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.20192826293372793</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1">
-        <f>SUM(C24:C29)</f>
-        <v>6251278</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.17513114174517244</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
-        <f>SUM(C18:C23)</f>
-        <v>5421695</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.10433415816278326</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C35">
+        <v>1794310</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="1">
+        <v>19</v>
+      </c>
+      <c r="C36">
+        <v>365546</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1">
-        <f>SUM(C15:C18)</f>
-        <v>3229968</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="1">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>365546</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16">
+      <c r="C37">
         <v>1969685</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B17">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38">
         <v>25</v>
       </c>
-      <c r="C17">
+      <c r="C38">
         <v>433529</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B18">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39">
         <v>26</v>
       </c>
-      <c r="C18">
+      <c r="C39">
         <v>461208</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B19" s="1">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B40" s="1">
         <v>27</v>
       </c>
-      <c r="C19">
+      <c r="C40">
         <v>480255</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B20">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41">
         <v>28</v>
       </c>
-      <c r="C20">
+      <c r="C41">
         <v>498849</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B21">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B42">
         <v>29</v>
       </c>
-      <c r="C21">
+      <c r="C42">
         <v>528880</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43">
         <v>2820162</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B23" s="4">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B44" s="5">
         <v>35</v>
       </c>
-      <c r="C23">
+      <c r="C44">
         <v>632341</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B24" s="3">
-        <v>36</v>
-      </c>
-      <c r="C24">
-        <v>651869</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B25" s="3">
-        <v>37</v>
-      </c>
-      <c r="C25">
-        <v>670804</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B26" s="3">
-        <v>38</v>
-      </c>
-      <c r="C26">
-        <v>649475</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B27" s="4">
-        <v>39</v>
-      </c>
-      <c r="C27">
-        <v>621242</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28">
-        <v>3075130</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B29" s="3">
-        <v>45</v>
-      </c>
-      <c r="C29">
-        <v>582758</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B30" s="3">
-        <v>46</v>
-      </c>
-      <c r="C30">
-        <v>560755</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B31" s="4">
-        <v>47</v>
-      </c>
-      <c r="C31">
-        <v>537782</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B32" s="4">
-        <v>48</v>
-      </c>
-      <c r="C32">
-        <v>516823</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B33" s="4">
-        <v>49</v>
-      </c>
-      <c r="C33">
-        <v>495123</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34">
-        <v>2282038</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B35" s="4">
-        <v>55</v>
-      </c>
-      <c r="C35">
-        <v>449985</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B36" s="4">
-        <v>56</v>
-      </c>
-      <c r="C36">
-        <v>458428</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B37" s="4">
-        <v>57</v>
-      </c>
-      <c r="C37">
-        <v>465903</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B38" s="4">
-        <v>58</v>
-      </c>
-      <c r="C38">
-        <v>467503</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B39" s="4">
-        <v>59</v>
-      </c>
-      <c r="C39">
-        <v>481609</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B40" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40">
-        <v>2680248</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B41" s="4">
-        <v>65</v>
-      </c>
-      <c r="C41">
-        <v>539691</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B42" s="4">
-        <v>66</v>
-      </c>
-      <c r="C42">
-        <v>511728</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B43" s="4">
-        <v>67</v>
-      </c>
-      <c r="C43">
-        <v>500838</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B44" s="4">
-        <v>68</v>
-      </c>
-      <c r="C44">
-        <v>484684</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" s="4">
+        <v>36</v>
+      </c>
+      <c r="C45">
+        <v>651869</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B46" s="4">
+        <v>37</v>
+      </c>
+      <c r="C46">
+        <v>670804</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B47" s="4">
+        <v>38</v>
+      </c>
+      <c r="C47">
+        <v>649475</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B48" s="5">
+        <v>39</v>
+      </c>
+      <c r="C48">
+        <v>621242</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>3075130</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B50" s="4">
+        <v>45</v>
+      </c>
+      <c r="C50">
+        <v>582758</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B51" s="4">
+        <v>46</v>
+      </c>
+      <c r="C51">
+        <v>560755</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B52" s="5">
+        <v>47</v>
+      </c>
+      <c r="C52">
+        <v>537782</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B53" s="5">
+        <v>48</v>
+      </c>
+      <c r="C53">
+        <v>516823</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B54" s="5">
+        <v>49</v>
+      </c>
+      <c r="C54">
+        <v>495123</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B55" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>2282038</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B56" s="5">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>449985</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B57" s="5">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>458428</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B58" s="5">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <v>465903</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B59" s="5">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <v>467503</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B60" s="5">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <v>481609</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61">
+        <v>2680248</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B62" s="5">
+        <v>65</v>
+      </c>
+      <c r="C62">
+        <v>539691</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B63" s="5">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>511728</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B64" s="5">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <v>500838</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" s="5">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>484684</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B66" s="5">
         <v>69</v>
       </c>
-      <c r="C45">
+      <c r="C66">
         <v>468654</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B46" s="3" t="s">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B67" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67">
+        <v>1916928</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B68" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C46">
-        <v>1916928</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B47" s="4" t="s">
+      <c r="C68">
+        <v>1013492</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B69" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C47">
-        <v>1013492</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B48" s="4" t="s">
+      <c r="C69">
+        <v>865717</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B70" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C48">
-        <v>865717</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B49" s="4" t="s">
+      <c r="C70">
+        <v>538356</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B71" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C49">
-        <v>538356</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B50" s="4" t="s">
+      <c r="C71">
+        <v>222498</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B72" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C50">
-        <v>222498</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B51" s="4" t="s">
+      <c r="C72">
+        <v>50517</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B73" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C51">
-        <v>50517</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B52" s="4" t="s">
+      <c r="C73">
+        <v>6882</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B74" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C52">
-        <v>6882</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B53" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53">
-        <f>SUM(C15:C52)</f>
+      <c r="C74">
+        <f>SUM(C36:C73)</f>
         <v>30957915</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B56" s="1"/>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B65" s="1"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B69" s="1"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B73" s="1"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B78" s="1"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.45">

</xml_diff>